<commit_message>
Room Db updated code added as meeitng_parser
Afftected table scheduler_rooms
</commit_message>
<xml_diff>
--- a/Extras/combined.xlsx
+++ b/Extras/combined.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wmich-my.sharepoint.com/personal/bdz9949_wmich_edu/Documents/Senior-Project/starter files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wmich-my.sharepoint.com/personal/mcg9062_wmich_edu/Documents/Desktop/senior_design/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{51C20BC9-3D00-4756-88D9-6E77FFA43A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C930830-BFBE-4C97-BB37-04C608150A60}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{51C20BC9-3D00-4756-88D9-6E77FFA43A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{F540CC54-3CAA-487A-A358-0057EE4D12A1}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8928" xr2:uid="{5451946F-3FDA-4E22-9745-D87473985FC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5451946F-3FDA-4E22-9745-D87473985FC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rooms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
-    <t>Rooms#</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Building</t>
   </si>
   <si>
@@ -157,6 +150,12 @@
   </si>
   <si>
     <t>E121</t>
+  </si>
+  <si>
+    <t>room_num</t>
+  </si>
+  <si>
+    <t>room_type</t>
   </si>
 </sst>
 </file>
@@ -511,529 +510,550 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E18">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E19">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E26">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E27">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E28">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E29">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E30">
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E32">
         <v>25</v>

</xml_diff>

<commit_message>
Added Header Information to Database
Changes are reflected in Rooms tables aswell
</commit_message>
<xml_diff>
--- a/Extras/combined.xlsx
+++ b/Extras/combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wmich-my.sharepoint.com/personal/mcg9062_wmich_edu/Documents/Desktop/senior_design/Extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{51C20BC9-3D00-4756-88D9-6E77FFA43A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{F540CC54-3CAA-487A-A358-0057EE4D12A1}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{51C20BC9-3D00-4756-88D9-6E77FFA43A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{45936C79-BA31-4DCE-9536-107994A4098E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5451946F-3FDA-4E22-9745-D87473985FC2}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="11970" windowHeight="8400" xr2:uid="{5451946F-3FDA-4E22-9745-D87473985FC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -152,10 +152,10 @@
     <t>E121</t>
   </si>
   <si>
-    <t>room_num</t>
-  </si>
-  <si>
-    <t>room_type</t>
+    <t>Room#</t>
+  </si>
+  <si>
+    <t>Room Type</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>